<commit_message>
clean up + Fitnesstracker
</commit_message>
<xml_diff>
--- a/Projects/WPMTracker/hWPM.xlsx
+++ b/Projects/WPMTracker/hWPM.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="13395" yWindow="4380" windowWidth="23700" windowHeight="15540" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="WPM" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="WPM" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -3914,7 +3914,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="63" t="n">
-        <v>44337.50060065928</v>
+        <v>44337.50060065973</v>
       </c>
       <c r="C89" s="64" t="n">
         <v>66</v>
@@ -3941,16 +3941,128 @@
       </c>
     </row>
     <row r="90">
-      <c r="B90" s="5" t="n"/>
+      <c r="A90" s="62" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="63" t="n">
+        <v>44338.38007898148</v>
+      </c>
+      <c r="C90" s="64" t="n">
+        <v>66</v>
+      </c>
+      <c r="D90" s="65" t="inlineStr">
+        <is>
+          <t>89.62</t>
+        </is>
+      </c>
+      <c r="E90" s="66" t="n">
+        <v>353</v>
+      </c>
+      <c r="F90" s="67" t="n">
+        <v>328</v>
+      </c>
+      <c r="G90" s="68" t="n">
+        <v>25</v>
+      </c>
+      <c r="H90" s="67" t="n">
+        <v>48</v>
+      </c>
+      <c r="I90" s="68" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="91">
-      <c r="B91" s="5" t="n"/>
+      <c r="A91" s="62" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="63" t="n">
+        <v>44340.44523178241</v>
+      </c>
+      <c r="C91" s="64" t="n">
+        <v>83</v>
+      </c>
+      <c r="D91" s="65" t="inlineStr">
+        <is>
+          <t>97.19</t>
+        </is>
+      </c>
+      <c r="E91" s="66" t="n">
+        <v>421</v>
+      </c>
+      <c r="F91" s="67" t="n">
+        <v>415</v>
+      </c>
+      <c r="G91" s="68" t="n">
+        <v>6</v>
+      </c>
+      <c r="H91" s="67" t="n">
+        <v>58</v>
+      </c>
+      <c r="I91" s="68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92">
-      <c r="B92" s="5" t="n"/>
+      <c r="A92" s="62" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="63" t="n">
+        <v>44340.44622471065</v>
+      </c>
+      <c r="C92" s="64" t="n">
+        <v>76</v>
+      </c>
+      <c r="D92" s="65" t="inlineStr">
+        <is>
+          <t>99.48</t>
+        </is>
+      </c>
+      <c r="E92" s="66" t="n">
+        <v>379</v>
+      </c>
+      <c r="F92" s="67" t="n">
+        <v>379</v>
+      </c>
+      <c r="G92" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" s="67" t="n">
+        <v>51</v>
+      </c>
+      <c r="I92" s="68" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
-      <c r="B93" s="5" t="n"/>
+      <c r="A93" s="62" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="63" t="n">
+        <v>44340.44698405136</v>
+      </c>
+      <c r="C93" s="64" t="n">
+        <v>73</v>
+      </c>
+      <c r="D93" s="65" t="inlineStr">
+        <is>
+          <t>94.59</t>
+        </is>
+      </c>
+      <c r="E93" s="66" t="n">
+        <v>373</v>
+      </c>
+      <c r="F93" s="67" t="n">
+        <v>367</v>
+      </c>
+      <c r="G93" s="68" t="n">
+        <v>6</v>
+      </c>
+      <c r="H93" s="67" t="n">
+        <v>49</v>
+      </c>
+      <c r="I93" s="68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" s="5" t="n"/>

</xml_diff>